<commit_message>
about to do some restructing
</commit_message>
<xml_diff>
--- a/connectionsTE.xlsx
+++ b/connectionsTE.xlsx
@@ -244,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +259,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -335,7 +341,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -350,6 +356,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -668,7 +676,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W51" sqref="W51"/>
+      <selection pane="topRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +846,7 @@
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5">
@@ -890,7 +898,7 @@
       <c r="AT2" s="5"/>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
@@ -942,7 +950,7 @@
       <c r="AT3" s="5"/>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5"/>
@@ -994,7 +1002,7 @@
       <c r="AT4" s="5"/>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5"/>
@@ -1046,7 +1054,7 @@
       <c r="AT5" s="5"/>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5"/>
@@ -1102,7 +1110,7 @@
       <c r="AT6" s="5"/>
     </row>
     <row r="7" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="5"/>
@@ -1154,7 +1162,7 @@
       <c r="AT7" s="5"/>
     </row>
     <row r="8" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="15" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="5"/>
@@ -1206,7 +1214,7 @@
       <c r="AT8" s="5"/>
     </row>
     <row r="9" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="5"/>
@@ -1258,7 +1266,7 @@
       <c r="AT9" s="5"/>
     </row>
     <row r="10" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="5"/>
@@ -1544,7 +1552,7 @@
       <c r="AT14" s="5"/>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="5"/>
@@ -1774,7 +1782,7 @@
       <c r="AT18" s="5"/>
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="5"/>
@@ -1944,7 +1952,7 @@
       <c r="AT21" s="5"/>
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="5"/>

</xml_diff>

<commit_message>
Algorithm changes wrt greedy pairing - slightly more readable. Connection matrix changed... There were some errors which affected the results. Need to go over the connection matrix again...
</commit_message>
<xml_diff>
--- a/connectionsTE.xlsx
+++ b/connectionsTE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="connections" sheetId="3" r:id="rId1"/>
@@ -521,9 +521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,8 +532,9 @@
     <col min="2" max="5" width="8.7109375" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -1700,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
@@ -1715,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="1">
         <v>0</v>
@@ -1809,7 +1810,7 @@
       </c>
       <c r="AZ8" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
@@ -1892,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="AA9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB9" s="1">
         <v>0</v>
@@ -1965,7 +1966,7 @@
       </c>
       <c r="AZ9" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
@@ -3596,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="W20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
@@ -3681,7 +3682,7 @@
       </c>
       <c r="AZ20" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
@@ -3707,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -3837,7 +3838,7 @@
       </c>
       <c r="AZ21" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
@@ -4019,7 +4020,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -4040,7 +4041,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
@@ -4058,7 +4059,7 @@
         <v>0</v>
       </c>
       <c r="U23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23" s="1">
         <v>0</v>
@@ -4149,7 +4150,7 @@
       </c>
       <c r="AZ23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
@@ -4175,10 +4176,10 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="1">
         <v>0</v>
@@ -4490,7 +4491,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="1">
         <v>0</v>
@@ -4617,7 +4618,7 @@
       </c>
       <c r="AZ26" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.25">
@@ -8374,7 +8375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="Z14" workbookViewId="0">
       <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
checked the flow sheets again made some changes
</commit_message>
<xml_diff>
--- a/connectionsTE.xlsx
+++ b/connectionsTE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="connections" sheetId="3" r:id="rId1"/>
-    <sheet name="exportme" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -521,9 +521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H26" sqref="H26"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="AZ15" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="1">
         <v>0</v>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="AZ17" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="1">
         <v>1</v>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="AZ18" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
@@ -3459,7 +3459,7 @@
         <v>0</v>
       </c>
       <c r="AC19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19" s="1">
         <v>0</v>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="AZ19" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
@@ -3594,7 +3594,7 @@
         <v>1</v>
       </c>
       <c r="V20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="1">
         <v>1</v>
@@ -3682,7 +3682,7 @@
       </c>
       <c r="AZ20" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
@@ -3708,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="AZ21" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
@@ -4056,7 +4056,7 @@
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="1">
         <v>1</v>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="AZ23" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
@@ -4179,7 +4179,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="1">
         <v>0</v>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="AZ24" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
@@ -4377,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="W25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X25" s="1">
         <v>0</v>
@@ -4462,7 +4462,7 @@
       </c>
       <c r="AZ25" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
@@ -4488,7 +4488,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
@@ -4533,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="W26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X26" s="1">
         <v>0</v>
@@ -4644,7 +4644,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -4695,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="Y27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z27" s="1">
         <v>0</v>
@@ -5121,7 +5121,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" s="1">
         <v>0</v>
@@ -5242,7 +5242,7 @@
       </c>
       <c r="AZ30" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
@@ -5280,7 +5280,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" s="1">
         <v>0</v>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="AZ31" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
@@ -8375,17 +8375,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX50"/>
   <sheetViews>
-    <sheetView topLeftCell="Z14" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -9490,7 +9490,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
@@ -9505,7 +9505,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="1">
         <v>0</v>
@@ -9678,7 +9678,7 @@
         <v>0</v>
       </c>
       <c r="AA9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB9" s="1">
         <v>0</v>
@@ -10533,7 +10533,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -10861,7 +10861,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="1">
         <v>0</v>
@@ -11013,7 +11013,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="1">
         <v>1</v>
@@ -11204,7 +11204,7 @@
         <v>0</v>
       </c>
       <c r="AC19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19" s="1">
         <v>0</v>
@@ -11335,10 +11335,10 @@
         <v>1</v>
       </c>
       <c r="V20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
@@ -11749,7 +11749,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -11770,13 +11770,13 @@
         <v>0</v>
       </c>
       <c r="O23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
@@ -11785,10 +11785,10 @@
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23" s="1">
         <v>0</v>
@@ -11901,7 +11901,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -12098,7 +12098,7 @@
         <v>0</v>
       </c>
       <c r="W25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X25" s="1">
         <v>0</v>
@@ -12205,10 +12205,10 @@
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="1">
         <v>0</v>
@@ -12250,7 +12250,7 @@
         <v>0</v>
       </c>
       <c r="W26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X26" s="1">
         <v>0</v>
@@ -12357,7 +12357,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -12408,7 +12408,7 @@
         <v>1</v>
       </c>
       <c r="Y27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z27" s="1">
         <v>0</v>
@@ -12822,7 +12822,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" s="1">
         <v>0</v>
@@ -12977,7 +12977,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
reverted to older connection matrices... its incredibly sensitive
</commit_message>
<xml_diff>
--- a/connectionsTE.xlsx
+++ b/connectionsTE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="connections" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="exportme" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -521,9 +521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD19" sqref="AD19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="AZ15" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="1">
         <v>0</v>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="AZ17" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="1">
         <v>1</v>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="AZ18" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
@@ -3459,7 +3459,7 @@
         <v>0</v>
       </c>
       <c r="AC19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD19" s="1">
         <v>0</v>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="AZ19" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
@@ -3594,7 +3594,7 @@
         <v>1</v>
       </c>
       <c r="V20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20" s="1">
         <v>1</v>
@@ -3682,7 +3682,7 @@
       </c>
       <c r="AZ20" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
@@ -3708,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="1">
         <v>0</v>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="AZ21" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
@@ -4056,7 +4056,7 @@
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="1">
         <v>1</v>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="AZ23" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
@@ -4179,7 +4179,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="1">
         <v>0</v>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="AZ24" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
@@ -4377,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="W25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X25" s="1">
         <v>0</v>
@@ -4462,7 +4462,7 @@
       </c>
       <c r="AZ25" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
@@ -4488,7 +4488,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
@@ -4533,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="W26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X26" s="1">
         <v>0</v>
@@ -4644,7 +4644,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -4695,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="Y27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z27" s="1">
         <v>0</v>
@@ -5121,7 +5121,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="1">
         <v>0</v>
@@ -5242,7 +5242,7 @@
       </c>
       <c r="AZ30" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
@@ -5280,7 +5280,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="1">
         <v>0</v>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="AZ31" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
@@ -8375,17 +8375,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="Z14" workbookViewId="0">
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -9490,7 +9490,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
@@ -9505,7 +9505,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="1">
         <v>0</v>
@@ -9678,7 +9678,7 @@
         <v>0</v>
       </c>
       <c r="AA9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB9" s="1">
         <v>0</v>
@@ -10533,7 +10533,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -10861,7 +10861,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="1">
         <v>0</v>
@@ -11013,7 +11013,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="1">
         <v>1</v>
@@ -11204,7 +11204,7 @@
         <v>0</v>
       </c>
       <c r="AC19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD19" s="1">
         <v>0</v>
@@ -11335,10 +11335,10 @@
         <v>1</v>
       </c>
       <c r="V20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
@@ -11749,7 +11749,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -11770,13 +11770,13 @@
         <v>0</v>
       </c>
       <c r="O23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
@@ -11785,10 +11785,10 @@
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V23" s="1">
         <v>0</v>
@@ -11901,7 +11901,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -12098,7 +12098,7 @@
         <v>0</v>
       </c>
       <c r="W25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X25" s="1">
         <v>0</v>
@@ -12205,10 +12205,10 @@
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="1">
         <v>0</v>
@@ -12250,7 +12250,7 @@
         <v>0</v>
       </c>
       <c r="W26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X26" s="1">
         <v>0</v>
@@ -12357,7 +12357,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -12408,7 +12408,7 @@
         <v>1</v>
       </c>
       <c r="Y27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z27" s="1">
         <v>0</v>
@@ -12822,7 +12822,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="1">
         <v>0</v>
@@ -12977,7 +12977,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="1">
         <v>0</v>

</xml_diff>